<commit_message>
Finalsim added SEB and SWB plots
</commit_message>
<xml_diff>
--- a/9_article1_FigsTables/Tables_data/res_mean_std.xlsx
+++ b/9_article1_FigsTables/Tables_data/res_mean_std.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\datamshapratirupa\9_article1_FigsTables\Tables_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F0586B-473F-459A-A868-530156994D4D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,8 +40,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,7 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -81,49 +75,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
       </left>
       <right style="thin">
         <color auto="1"/>
@@ -136,92 +89,26 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -263,7 +150,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,27 +182,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -347,24 +216,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,85 +391,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5">
-        <v>0.96099999999999997</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2">
+        <v>0.961</v>
+      </c>
+      <c r="C2">
         <v>1.821</v>
       </c>
-      <c r="D2" s="5">
-        <v>3.0939999999999999</v>
-      </c>
-      <c r="E2" s="6">
-        <v>8.8740000000000006</v>
+      <c r="D2">
+        <v>3.094</v>
+      </c>
+      <c r="E2">
+        <v>8.874000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5">
-        <v>0.47399999999999998</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2.0430000000000001</v>
-      </c>
-      <c r="D3" s="5">
-        <v>-0.83199999999999996</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="B3">
+        <v>0.474</v>
+      </c>
+      <c r="C3">
+        <v>2.043</v>
+      </c>
+      <c r="D3">
+        <v>-0.832</v>
+      </c>
+      <c r="E3">
         <v>5.59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4">
         <v>0.121</v>
       </c>
-      <c r="C4" s="8">
-        <v>4.4080000000000004</v>
-      </c>
-      <c r="D4" s="8">
-        <v>6.2910000000000004</v>
-      </c>
-      <c r="E4" s="9">
+      <c r="C4">
+        <v>4.408</v>
+      </c>
+      <c r="D4">
+        <v>6.291</v>
+      </c>
+      <c r="E4">
         <v>10.914</v>
       </c>
     </row>

</xml_diff>